<commit_message>
t: move common code into utils library
</commit_message>
<xml_diff>
--- a/t/data/clone-easy.xlsx
+++ b/t/data/clone-easy.xlsx
@@ -438,9 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -475,9 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>

</xml_diff>